<commit_message>
updated product_added, added view product page
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -38,10 +38,19 @@
     <t>Strain Type</t>
   </si>
   <si>
+    <t>Strain Terpenes</t>
+  </si>
+  <si>
+    <t>Strain Taste</t>
+  </si>
+  <si>
     <t>THC %</t>
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
   <si>
     <t>Main Image</t>
@@ -773,6 +782,7 @@
     <col customWidth="1" min="1" max="1" width="23.0"/>
     <col customWidth="1" min="2" max="2" width="90.25"/>
     <col customWidth="1" min="6" max="6" width="14.63"/>
+    <col customWidth="1" min="9" max="9" width="13.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -830,28 +840,37 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E2" s="4">
         <v>39.0</v>
@@ -860,364 +879,376 @@
         <v>35.0</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="4">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4">
         <v>84.7</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="S2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4">
         <v>25.0</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>32</v>
+      <c r="L3" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4" s="4">
         <v>25.0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="4">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
         <v>92.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E5" s="4">
         <v>20.0</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>41</v>
+      <c r="L5" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E6" s="4">
         <v>35.0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="4">
+        <v>39</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
         <v>85.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4">
         <v>30.0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="4">
+        <v>51</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4">
         <v>5.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4">
         <v>35.0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="4">
+        <v>55</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
         <v>17.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" s="4">
         <v>55.0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="4">
+        <v>57</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
         <v>21.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="4">
+        <v>63</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4">
         <v>100.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="4">
+        <v>67</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4">
         <v>19.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="4">
+        <v>74</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4">
         <v>50.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="4">
+        <v>77</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4">
         <v>100.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="4">
+        <v>80</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4">
         <v>6.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I18" s="4">
+        <v>86</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4">
         <v>500.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
@@ -4184,34 +4215,34 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
@@ -4219,486 +4250,486 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4">
         <v>18.0</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C3" s="4">
         <v>18.0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4">
         <v>19.0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4">
         <v>20.0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C6" s="4">
         <v>24.0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C7" s="4">
         <v>19.0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C8" s="4">
         <v>20.0</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4">
         <v>20.0</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C10" s="4">
         <v>20.0</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4">
         <v>23.0</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="M11" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C12" s="4">
         <v>22.0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C13" s="4">
         <v>19.0</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C14" s="4">
         <v>25.0</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C15" s="4">
         <v>23.0</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C16" s="4">
         <v>23.0</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C17" s="4">
         <v>23.0</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4">
         <v>18.0</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="M18" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C19" s="4">
         <v>19.0</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4">
         <v>21.0</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C21" s="4">
         <v>21.0</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>